<commit_message>
valuationProcess method file added.
</commit_message>
<xml_diff>
--- a/uploads/FCFE_Template.xlsx
+++ b/uploads/FCFE_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shahnawaz/Documents/ifinworth/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ifinworth\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A24F0792-9DD4-964A-9DCD-CBC8BFF7D068}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC566B3C-B8D3-4595-8698-D8470C4A8FA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15800" activeTab="1" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{11B12A5D-7249-4041-8AA7-3E354D49454B}"/>
   </bookViews>
   <sheets>
     <sheet name="P&amp;L" sheetId="1" r:id="rId1"/>
@@ -24,22 +24,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="117">
   <si>
     <t>Revenue from Operations</t>
   </si>
@@ -373,6 +363,24 @@
   </si>
   <si>
     <t>Y6</t>
+  </si>
+  <si>
+    <t>2023-2024</t>
+  </si>
+  <si>
+    <t>2024-2025</t>
+  </si>
+  <si>
+    <t>2025-2026</t>
+  </si>
+  <si>
+    <t>2026-2027</t>
+  </si>
+  <si>
+    <t>2027-2028</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Provisionals/Audited Nos. close to valuation, 2022-2023</t>
   </si>
 </sst>
 </file>
@@ -380,8 +388,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="166" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
@@ -720,12 +728,12 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -817,7 +825,7 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -880,57 +888,15 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="7" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="16" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="7" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="11" fillId="5" borderId="16" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -938,6 +904,45 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="3" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="3" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="7" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="16" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="6" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="7" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="5" borderId="16" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="3" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -960,43 +965,13 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
-      <sheetName val="P&amp;L"/>
-      <sheetName val="BS"/>
       <sheetName val="Sheet2"/>
-      <sheetName val="Excess Earnings Model"/>
-      <sheetName val="FCFF"/>
-      <sheetName val="FCFE"/>
-      <sheetName val="Relative Valuation"/>
-      <sheetName val="Comparable Trans Multiple"/>
-      <sheetName val="Net Asset Value"/>
-      <sheetName val="SOTP"/>
-      <sheetName val="Black Scholes"/>
-      <sheetName val="Weighted Valuation"/>
-      <sheetName val="Sheet1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0"/>
-      <sheetData sheetId="1"/>
-      <sheetData sheetId="2">
-        <row r="11">
-          <cell r="C11" t="str">
-            <v>Ask user for same</v>
-          </cell>
-        </row>
-      </sheetData>
-      <sheetData sheetId="3"/>
-      <sheetData sheetId="4"/>
-      <sheetData sheetId="5"/>
-      <sheetData sheetId="6"/>
-      <sheetData sheetId="7"/>
-      <sheetData sheetId="8"/>
-      <sheetData sheetId="9"/>
-      <sheetData sheetId="10"/>
-      <sheetData sheetId="11"/>
-      <sheetData sheetId="12"/>
+      <sheetData sheetId="0" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -1301,76 +1276,76 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{20D100AD-1EC3-3246-AFE5-16D06F619914}">
   <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="57.19921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="36.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
+    <row r="1" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="69" t="s">
         <v>97</v>
       </c>
-      <c r="B1" s="65" t="s">
-        <v>105</v>
+      <c r="B1" s="71" t="s">
+        <v>116</v>
       </c>
       <c r="C1" s="68" t="s">
-        <v>106</v>
-      </c>
-      <c r="D1" s="74" t="s">
-        <v>107</v>
-      </c>
-      <c r="E1" s="75" t="s">
-        <v>108</v>
-      </c>
-      <c r="F1" s="76" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" s="76" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="64"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-    </row>
-    <row r="3" spans="1:7" ht="17" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="64"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="74"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="76"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="D1" s="68" t="s">
+        <v>112</v>
+      </c>
+      <c r="E1" s="68" t="s">
+        <v>113</v>
+      </c>
+      <c r="F1" s="68" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="68" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="70"/>
+      <c r="B2" s="71"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="68"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="70"/>
+      <c r="B3" s="71"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="68"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="68"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="2"/>
       <c r="B4" s="28"/>
       <c r="C4" s="54"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="28"/>
       <c r="C5" s="54"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
       <c r="B6" s="28"/>
       <c r="C6" s="54"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>98</v>
       </c>
@@ -1394,7 +1369,7 @@
         <v>784791956.28016102</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>1</v>
       </c>
@@ -1418,7 +1393,7 @@
         <v>742882.97659472644</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="4" t="s">
         <v>0</v>
       </c>
@@ -1442,24 +1417,24 @@
         <v>785534839.25675571</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="28"/>
       <c r="C10" s="54"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B11" s="28"/>
       <c r="C11" s="54"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="2"/>
       <c r="B12" s="28"/>
       <c r="C12" s="54"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
         <v>3</v>
       </c>
@@ -1480,7 +1455,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
         <v>4</v>
       </c>
@@ -1504,7 +1479,7 @@
         <v>431635575.95408857</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
         <v>5</v>
       </c>
@@ -1528,7 +1503,7 @@
         <v>15695839.125603221</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
         <v>6</v>
       </c>
@@ -1551,49 +1526,49 @@
         <v>202736531.03407711</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B17" s="28"/>
       <c r="C17" s="54"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="28"/>
       <c r="C18" s="54"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="28"/>
       <c r="C19" s="54"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="28"/>
       <c r="C20" s="54"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="28"/>
       <c r="C21" s="54"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="28"/>
       <c r="C22" s="54"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="2" t="s">
         <v>13</v>
       </c>
@@ -1616,12 +1591,12 @@
         <v>202736531.03407711</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="2"/>
       <c r="B24" s="28"/>
       <c r="C24" s="54"/>
     </row>
-    <row r="25" spans="1:7" ht="28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="26.4" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>14</v>
       </c>
@@ -1645,7 +1620,7 @@
         <v>135466893.14298683</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="42" t="s">
         <v>15</v>
       </c>
@@ -1668,7 +1643,7 @@
         <v>29513574.700000003</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
         <v>16</v>
       </c>
@@ -1692,7 +1667,7 @@
         <v>105953318.44298683</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
         <v>17</v>
       </c>
@@ -1715,12 +1690,12 @@
         <v>23171362.692883004</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="28" t="s">
-        <v>99</v>
+      <c r="B29" s="32">
+        <v>7</v>
       </c>
       <c r="C29" s="54">
         <v>0</v>
@@ -1735,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>19</v>
       </c>
@@ -1759,12 +1734,12 @@
         <v>82781955.750103831</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="44" t="s">
         <v>20</v>
       </c>
-      <c r="B31" s="28" t="s">
-        <v>99</v>
+      <c r="B31" s="28">
+        <v>2</v>
       </c>
       <c r="C31" s="54">
         <v>0</v>
@@ -1779,7 +1754,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="7" t="s">
         <v>21</v>
       </c>
@@ -1803,11 +1778,11 @@
         <v>82781955.750103831</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="28" t="s">
+      <c r="B33" s="32" t="s">
         <v>99</v>
       </c>
       <c r="C33" s="54">
@@ -1823,7 +1798,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="8" t="s">
         <v>23</v>
       </c>
@@ -1847,7 +1822,7 @@
         <v>82781955.750103831</v>
       </c>
     </row>
-    <row r="35" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>24</v>
       </c>
@@ -1871,7 +1846,7 @@
         <v>24834586.725031149</v>
       </c>
     </row>
-    <row r="36" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="9" t="s">
         <v>25</v>
       </c>
@@ -1894,7 +1869,7 @@
         <v>24834586.725031149</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="9" t="s">
         <v>26</v>
       </c>
@@ -1914,7 +1889,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A38" s="9" t="s">
         <v>27</v>
       </c>
@@ -1934,7 +1909,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="9" t="s">
         <v>28</v>
       </c>
@@ -1954,7 +1929,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="9" t="s">
         <v>29</v>
       </c>
@@ -1974,12 +1949,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="7"/>
       <c r="B41" s="35"/>
       <c r="C41" s="60"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>30</v>
       </c>
@@ -2003,19 +1978,19 @@
         <v>57947369.025072679</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="7"/>
       <c r="B43" s="35"/>
       <c r="C43" s="60"/>
     </row>
-    <row r="44" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>31</v>
       </c>
       <c r="B44" s="35"/>
       <c r="C44" s="60"/>
     </row>
-    <row r="45" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="10" t="s">
         <v>32</v>
       </c>
@@ -2035,7 +2010,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="29" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="6" t="s">
         <v>33</v>
       </c>
@@ -2055,12 +2030,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A47" s="6"/>
       <c r="B47" s="35"/>
       <c r="C47" s="60"/>
     </row>
-    <row r="48" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="10" t="s">
         <v>34</v>
       </c>
@@ -2080,7 +2055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="9" t="s">
         <v>35</v>
       </c>
@@ -2100,7 +2075,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="9" t="s">
         <v>36</v>
       </c>
@@ -2120,12 +2095,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="37"/>
       <c r="B51" s="34"/>
       <c r="C51" s="56"/>
     </row>
-    <row r="52" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="7" t="s">
         <v>37</v>
       </c>
@@ -2145,12 +2120,12 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="37"/>
       <c r="B53" s="35"/>
       <c r="C53" s="60"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="8" t="s">
         <v>38</v>
       </c>
@@ -2174,28 +2149,28 @@
         <v>57947369.025072679</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="37" t="s">
         <v>100</v>
       </c>
       <c r="B55" s="35"/>
       <c r="C55" s="60"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="37" t="s">
         <v>101</v>
       </c>
       <c r="B56" s="35"/>
       <c r="C56" s="60"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="38" t="s">
         <v>102</v>
       </c>
       <c r="B57" s="27"/>
       <c r="C57" s="26"/>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="37" t="s">
         <v>103</v>
       </c>
@@ -2234,59 +2209,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2ABB34C2-FC5D-EB4C-A739-CF87FCBB2D79}">
   <dimension ref="A1:G76"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="79.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="79.19921875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="7" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="12.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="71" t="s">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" s="75" t="s">
         <v>96</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="78" t="s">
         <v>105</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="72" t="s">
         <v>106</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="72" t="s">
         <v>107</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="G1" s="68" t="s">
+      <c r="G1" s="72" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="72"/>
-      <c r="B2" s="66"/>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-    </row>
-    <row r="3" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="73"/>
-      <c r="B3" s="67"/>
-      <c r="C3" s="70"/>
-      <c r="D3" s="70"/>
-      <c r="E3" s="70"/>
-      <c r="F3" s="70"/>
-      <c r="G3" s="70"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="76"/>
+      <c r="B2" s="79"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+    </row>
+    <row r="3" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="77"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="74"/>
+      <c r="D3" s="74"/>
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>39</v>
       </c>
@@ -2296,7 +2271,7 @@
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="13"/>
       <c r="B5" s="12"/>
       <c r="C5" s="12"/>
@@ -2304,7 +2279,7 @@
       <c r="E5" s="12"/>
       <c r="F5" s="12"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>40</v>
       </c>
@@ -2333,7 +2308,7 @@
         <v>250147669.6013369</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>41</v>
       </c>
@@ -2356,7 +2331,7 @@
         <v>33800000</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="15" t="s">
         <v>42</v>
       </c>
@@ -2376,7 +2351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="17" t="s">
         <v>43</v>
       </c>
@@ -2396,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="15" t="s">
         <v>44</v>
       </c>
@@ -2416,7 +2391,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="15" t="s">
         <v>45</v>
       </c>
@@ -2439,7 +2414,7 @@
         <v>216347669.6013369</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="15" t="s">
         <v>46</v>
       </c>
@@ -2459,7 +2434,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="15" t="s">
         <v>47</v>
       </c>
@@ -2479,7 +2454,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="15" t="s">
         <v>48</v>
       </c>
@@ -2499,7 +2474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="15" t="s">
         <v>49</v>
       </c>
@@ -2509,7 +2484,7 @@
       <c r="E15" s="16"/>
       <c r="F15" s="16"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="15" t="s">
         <v>50</v>
       </c>
@@ -2529,7 +2504,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" s="15" t="s">
         <v>51</v>
       </c>
@@ -2539,7 +2514,7 @@
       <c r="E17" s="16"/>
       <c r="F17" s="16"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" s="15" t="s">
         <v>52</v>
       </c>
@@ -2562,7 +2537,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="15" t="s">
         <v>53</v>
       </c>
@@ -2585,7 +2560,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="15"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2594,7 +2569,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="17" t="s">
         <v>54</v>
       </c>
@@ -2605,7 +2580,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" s="17" t="s">
         <v>55</v>
       </c>
@@ -2628,7 +2603,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" s="17"/>
       <c r="B23" s="16">
         <v>0</v>
@@ -2649,7 +2624,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>56</v>
       </c>
@@ -2678,7 +2653,7 @@
         <v>147115025.78</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" s="46" t="s">
         <v>57</v>
       </c>
@@ -2701,7 +2676,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" s="15"/>
       <c r="B26" s="16">
         <v>0</v>
@@ -2722,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" s="46" t="s">
         <v>58</v>
       </c>
@@ -2745,7 +2720,7 @@
         <v>147115025.78</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
         <v>59</v>
       </c>
@@ -2755,7 +2730,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="16"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" s="15" t="s">
         <v>60</v>
       </c>
@@ -2778,7 +2753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" s="15" t="s">
         <v>61</v>
       </c>
@@ -2798,7 +2773,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" s="15" t="s">
         <v>62</v>
       </c>
@@ -2818,7 +2793,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" s="15"/>
       <c r="B32" s="16"/>
       <c r="C32" s="16"/>
@@ -2826,7 +2801,7 @@
       <c r="E32" s="16"/>
       <c r="F32" s="16"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="13" t="s">
         <v>63</v>
       </c>
@@ -2855,7 +2830,7 @@
         <v>474009946.91888213</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="15" t="s">
         <v>64</v>
       </c>
@@ -2878,7 +2853,7 @@
         <v>118256322.17920235</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="15" t="s">
         <v>65</v>
       </c>
@@ -2898,7 +2873,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" s="15" t="s">
         <v>66</v>
       </c>
@@ -2921,7 +2896,7 @@
         <v>17180255.309999999</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" s="15" t="s">
         <v>67</v>
       </c>
@@ -2941,7 +2916,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" s="15" t="s">
         <v>68</v>
       </c>
@@ -2964,35 +2939,35 @@
         <v>318817761.42967981</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" s="15" t="s">
         <v>69</v>
       </c>
       <c r="B39" s="3">
         <v>19755608</v>
       </c>
-      <c r="C39" s="77">
+      <c r="C39" s="63">
         <f>+B39</f>
         <v>19755608</v>
       </c>
-      <c r="D39" s="77">
+      <c r="D39" s="63">
         <f t="shared" ref="D39:G39" si="3">+C39</f>
         <v>19755608</v>
       </c>
-      <c r="E39" s="77">
+      <c r="E39" s="63">
         <f t="shared" si="3"/>
         <v>19755608</v>
       </c>
-      <c r="F39" s="77">
+      <c r="F39" s="63">
         <f t="shared" si="3"/>
         <v>19755608</v>
       </c>
-      <c r="G39" s="77">
+      <c r="G39" s="63">
         <f t="shared" si="3"/>
         <v>19755608</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>70</v>
       </c>
@@ -3002,7 +2977,7 @@
       <c r="E40" s="19"/>
       <c r="F40" s="19"/>
     </row>
-    <row r="41" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A41" s="21" t="s">
         <v>71</v>
       </c>
@@ -3031,7 +3006,7 @@
         <v>871272642.30021906</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="15"/>
       <c r="B42" s="19"/>
       <c r="C42" s="19"/>
@@ -3039,7 +3014,7 @@
       <c r="E42" s="19"/>
       <c r="F42" s="19"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="13" t="s">
         <v>72</v>
       </c>
@@ -3049,7 +3024,7 @@
       <c r="E43" s="19"/>
       <c r="F43" s="19"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="13"/>
       <c r="B44" s="19"/>
       <c r="C44" s="19"/>
@@ -3057,7 +3032,7 @@
       <c r="E44" s="19"/>
       <c r="F44" s="19"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" s="17" t="s">
         <v>73</v>
       </c>
@@ -3086,7 +3061,7 @@
         <v>625465978.29999995</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" s="53" t="s">
         <v>74</v>
       </c>
@@ -3115,7 +3090,7 @@
         <v>501647574.30000001</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" s="13" t="s">
         <v>75</v>
       </c>
@@ -3125,7 +3100,7 @@
       <c r="E47" s="16"/>
       <c r="F47" s="16"/>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" s="23" t="s">
         <v>76</v>
       </c>
@@ -3148,7 +3123,7 @@
         <v>501647574.30000001</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" s="23" t="s">
         <v>77</v>
       </c>
@@ -3168,7 +3143,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" s="23" t="s">
         <v>78</v>
       </c>
@@ -3188,7 +3163,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" s="23" t="s">
         <v>79</v>
       </c>
@@ -3208,7 +3183,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" s="23" t="s">
         <v>80</v>
       </c>
@@ -3228,7 +3203,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" s="23" t="s">
         <v>81</v>
       </c>
@@ -3248,7 +3223,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" s="23"/>
       <c r="B54" s="16"/>
       <c r="C54" s="16"/>
@@ -3256,7 +3231,7 @@
       <c r="E54" s="16"/>
       <c r="F54" s="16"/>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" s="23" t="s">
         <v>82</v>
       </c>
@@ -3276,30 +3251,30 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" s="48" t="s">
         <v>83</v>
       </c>
       <c r="B56" s="3">
         <v>29770092</v>
       </c>
-      <c r="C56" s="78">
+      <c r="C56" s="64">
         <v>29770092</v>
       </c>
-      <c r="D56" s="78">
+      <c r="D56" s="64">
         <v>29770092</v>
       </c>
-      <c r="E56" s="78">
+      <c r="E56" s="64">
         <v>29770092</v>
       </c>
-      <c r="F56" s="78">
+      <c r="F56" s="64">
         <v>29770092</v>
       </c>
-      <c r="G56" s="78">
+      <c r="G56" s="64">
         <v>29770092</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" s="15" t="s">
         <v>84</v>
       </c>
@@ -3319,7 +3294,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" s="15" t="s">
         <v>85</v>
       </c>
@@ -3342,35 +3317,35 @@
         <v>92251687</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" s="46" t="s">
         <v>86</v>
       </c>
       <c r="B59" s="24">
         <v>1796625</v>
       </c>
-      <c r="C59" s="79">
+      <c r="C59" s="65">
         <f>+B59</f>
         <v>1796625</v>
       </c>
-      <c r="D59" s="79">
+      <c r="D59" s="65">
         <f t="shared" ref="D59:G59" si="8">+C59</f>
         <v>1796625</v>
       </c>
-      <c r="E59" s="79">
+      <c r="E59" s="65">
         <f t="shared" si="8"/>
         <v>1796625</v>
       </c>
-      <c r="F59" s="79">
+      <c r="F59" s="65">
         <f t="shared" si="8"/>
         <v>1796625</v>
       </c>
-      <c r="G59" s="79">
+      <c r="G59" s="65">
         <f t="shared" si="8"/>
         <v>1796625</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" s="15"/>
       <c r="B60" s="16"/>
       <c r="C60" s="16"/>
@@ -3378,7 +3353,7 @@
       <c r="E60" s="16"/>
       <c r="F60" s="16"/>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" s="17" t="s">
         <v>87</v>
       </c>
@@ -3407,7 +3382,7 @@
         <v>245806663.99556866</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" s="46" t="s">
         <v>88</v>
       </c>
@@ -3430,7 +3405,7 @@
         <v>12494552.641662903</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" s="46" t="s">
         <v>89</v>
       </c>
@@ -3450,7 +3425,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" s="46" t="s">
         <v>90</v>
       </c>
@@ -3473,7 +3448,7 @@
         <v>32251724.230691548</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" s="46" t="s">
         <v>91</v>
       </c>
@@ -3493,7 +3468,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" s="48" t="s">
         <v>92</v>
       </c>
@@ -3516,79 +3491,79 @@
         <v>104656711.12321422</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" s="49" t="s">
         <v>93</v>
       </c>
       <c r="B67" s="50">
         <v>87608143</v>
       </c>
-      <c r="C67" s="80">
+      <c r="C67" s="66">
         <v>87608143</v>
       </c>
-      <c r="D67" s="80">
+      <c r="D67" s="66">
         <v>87608143</v>
       </c>
-      <c r="E67" s="80">
+      <c r="E67" s="66">
         <v>77608143</v>
       </c>
-      <c r="F67" s="80">
+      <c r="F67" s="66">
         <v>77608143</v>
       </c>
-      <c r="G67" s="81">
+      <c r="G67" s="67">
         <v>77608143</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" s="49" t="s">
         <v>94</v>
       </c>
       <c r="B68" s="50">
         <v>0</v>
       </c>
-      <c r="C68" s="80">
-        <v>0</v>
-      </c>
-      <c r="D68" s="80">
-        <v>0</v>
-      </c>
-      <c r="E68" s="80">
-        <v>0</v>
-      </c>
-      <c r="F68" s="80">
-        <v>0</v>
-      </c>
-      <c r="G68" s="81"/>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="C68" s="66">
+        <v>0</v>
+      </c>
+      <c r="D68" s="66">
+        <v>0</v>
+      </c>
+      <c r="E68" s="66">
+        <v>0</v>
+      </c>
+      <c r="F68" s="66">
+        <v>0</v>
+      </c>
+      <c r="G68" s="67"/>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" s="51" t="s">
         <v>95</v>
       </c>
       <c r="B69" s="52">
         <v>18795533</v>
       </c>
-      <c r="C69" s="78">
+      <c r="C69" s="64">
         <f>+B69</f>
         <v>18795533</v>
       </c>
-      <c r="D69" s="78">
+      <c r="D69" s="64">
         <f t="shared" ref="D69:G69" si="10">+C69</f>
         <v>18795533</v>
       </c>
-      <c r="E69" s="78">
+      <c r="E69" s="64">
         <f t="shared" si="10"/>
         <v>18795533</v>
       </c>
-      <c r="F69" s="78">
+      <c r="F69" s="64">
         <f t="shared" si="10"/>
         <v>18795533</v>
       </c>
-      <c r="G69" s="78">
+      <c r="G69" s="64">
         <f t="shared" si="10"/>
         <v>18795533</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" s="15"/>
       <c r="B70" s="16"/>
       <c r="C70" s="16"/>
@@ -3596,7 +3571,7 @@
       <c r="E70" s="16"/>
       <c r="F70" s="16"/>
     </row>
-    <row r="71" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A71" s="15"/>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
@@ -3604,7 +3579,7 @@
       <c r="E71" s="25"/>
       <c r="F71" s="25"/>
     </row>
-    <row r="72" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A72" s="21" t="s">
         <v>71</v>
       </c>
@@ -3633,13 +3608,13 @@
         <v>871272642.29556859</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B74" s="40">
         <f>+B72-B41</f>
         <v>-0.54999995231628418</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>104</v>
       </c>

</xml_diff>